<commit_message>
完成 LL1 语法分析 1. 实现 ll1 算法，完成 first sets、follow sets 、predict table 的求解。内容存放在 ll1 类中 2. ImplAdapter 实现抽象类 AbstractSyntaxerImpl,将其中的抽象方法委托给 ll1 类 3.  CoreAdapter 实现抽象类 AbstractSyntaxerCore ，其中的 analyze 方法委托给，ll1 类中 doLL1 方法实现
</commit_message>
<xml_diff>
--- a/src/main/resources/default/defaultToken.xlsx
+++ b/src/main/resources/default/defaultToken.xlsx
@@ -137,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyBorder="true" applyFill="true" applyFont="true">
       <alignment horizontal="center" wrapText="true" vertical="center"/>
@@ -189,7 +189,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
@@ -230,7 +229,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C81"/>
+  <dimension ref="A1:C80"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -930,16 +929,16 @@
     </row>
     <row r="47">
       <c r="A47" s="48" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="B47" s="48" t="inlineStr">
         <is>
-          <t>ENDDELIMITER/SEMICOLON</t>
+          <t>WHITESPACE/NEW_LINE</t>
         </is>
       </c>
       <c r="C47" s="48" t="inlineStr">
         <is>
-          <t>;</t>
+          <t>\n</t>
         </is>
       </c>
     </row>
@@ -949,12 +948,12 @@
       </c>
       <c r="B48" s="49" t="inlineStr">
         <is>
-          <t>WHITESPACE/NEW_LINE</t>
+          <t>WHITESPACE/SPACE</t>
         </is>
       </c>
       <c r="C48" s="49" t="inlineStr">
         <is>
-          <t>\n</t>
+          <t>空格</t>
         </is>
       </c>
     </row>
@@ -1009,12 +1008,12 @@
       </c>
       <c r="B52" s="53" t="inlineStr">
         <is>
-          <t>WHITESPACE/SPACE</t>
+          <t>IDENTIFIER</t>
         </is>
       </c>
       <c r="C52" s="53" t="inlineStr">
         <is>
-          <t>空格</t>
+          <t>v1</t>
         </is>
       </c>
     </row>
@@ -1024,12 +1023,12 @@
       </c>
       <c r="B53" s="54" t="inlineStr">
         <is>
-          <t>IDENTIFIER</t>
+          <t>WHITESPACE/SPACE</t>
         </is>
       </c>
       <c r="C53" s="54" t="inlineStr">
         <is>
-          <t>v1</t>
+          <t>空格</t>
         </is>
       </c>
     </row>
@@ -1039,12 +1038,12 @@
       </c>
       <c r="B54" s="55" t="inlineStr">
         <is>
-          <t>WHITESPACE/SPACE</t>
+          <t>DOUBLECHARDELIMITER/ASSIGN</t>
         </is>
       </c>
       <c r="C54" s="55" t="inlineStr">
         <is>
-          <t>空格</t>
+          <t>:=</t>
         </is>
       </c>
     </row>
@@ -1054,12 +1053,12 @@
       </c>
       <c r="B55" s="56" t="inlineStr">
         <is>
-          <t>DOUBLECHARDELIMITER/ASSIGN</t>
+          <t>WHITESPACE/SPACE</t>
         </is>
       </c>
       <c r="C55" s="56" t="inlineStr">
         <is>
-          <t>:=</t>
+          <t>空格</t>
         </is>
       </c>
     </row>
@@ -1069,12 +1068,12 @@
       </c>
       <c r="B56" s="57" t="inlineStr">
         <is>
-          <t>WHITESPACE/SPACE</t>
+          <t>IDENTIFIER</t>
         </is>
       </c>
       <c r="C56" s="57" t="inlineStr">
         <is>
-          <t>空格</t>
+          <t>v1</t>
         </is>
       </c>
     </row>
@@ -1084,12 +1083,12 @@
       </c>
       <c r="B57" s="58" t="inlineStr">
         <is>
-          <t>IDENTIFIER</t>
+          <t>WHITESPACE/SPACE</t>
         </is>
       </c>
       <c r="C57" s="58" t="inlineStr">
         <is>
-          <t>v1</t>
+          <t>空格</t>
         </is>
       </c>
     </row>
@@ -1099,12 +1098,12 @@
       </c>
       <c r="B58" s="59" t="inlineStr">
         <is>
-          <t>WHITESPACE/SPACE</t>
+          <t>OPERATOR/PLUS</t>
         </is>
       </c>
       <c r="C58" s="59" t="inlineStr">
         <is>
-          <t>空格</t>
+          <t>+</t>
         </is>
       </c>
     </row>
@@ -1114,12 +1113,12 @@
       </c>
       <c r="B59" s="60" t="inlineStr">
         <is>
-          <t>OPERATOR/PLUS</t>
+          <t>WHITESPACE/SPACE</t>
         </is>
       </c>
       <c r="C59" s="60" t="inlineStr">
         <is>
-          <t>+</t>
+          <t>空格</t>
         </is>
       </c>
     </row>
@@ -1129,12 +1128,12 @@
       </c>
       <c r="B60" s="61" t="inlineStr">
         <is>
-          <t>WHITESPACE/SPACE</t>
+          <t>CONSTANT/UNSIGNED_INTEGER</t>
         </is>
       </c>
       <c r="C60" s="61" t="inlineStr">
         <is>
-          <t>空格</t>
+          <t>10</t>
         </is>
       </c>
     </row>
@@ -1144,27 +1143,27 @@
       </c>
       <c r="B61" s="62" t="inlineStr">
         <is>
-          <t>CONSTANT/UNSIGNED_INTEGER</t>
+          <t>ENDDELIMITER/SEMICOLON</t>
         </is>
       </c>
       <c r="C61" s="62" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>;</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="63" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
       <c r="B62" s="63" t="inlineStr">
         <is>
-          <t>ENDDELIMITER/SEMICOLON</t>
+          <t>WHITESPACE/NEW_LINE</t>
         </is>
       </c>
       <c r="C62" s="63" t="inlineStr">
         <is>
-          <t>;</t>
+          <t>\n</t>
         </is>
       </c>
     </row>
@@ -1174,12 +1173,12 @@
       </c>
       <c r="B63" s="64" t="inlineStr">
         <is>
-          <t>WHITESPACE/NEW_LINE</t>
+          <t>WHITESPACE/SPACE</t>
         </is>
       </c>
       <c r="C63" s="64" t="inlineStr">
         <is>
-          <t>\n</t>
+          <t>空格</t>
         </is>
       </c>
     </row>
@@ -1234,27 +1233,27 @@
       </c>
       <c r="B67" s="68" t="inlineStr">
         <is>
-          <t>WHITESPACE/SPACE</t>
+          <t>COMMENT</t>
         </is>
       </c>
       <c r="C67" s="68" t="inlineStr">
         <is>
-          <t>空格</t>
+          <t>{write('a'')}</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="69" t="n">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="B68" s="69" t="inlineStr">
         <is>
-          <t>COMMENT</t>
+          <t>WHITESPACE/NEW_LINE</t>
         </is>
       </c>
       <c r="C68" s="69" t="inlineStr">
         <is>
-          <t>{write('a'')}</t>
+          <t>\n</t>
         </is>
       </c>
     </row>
@@ -1264,12 +1263,12 @@
       </c>
       <c r="B69" s="70" t="inlineStr">
         <is>
-          <t>WHITESPACE/NEW_LINE</t>
+          <t>WHITESPACE/SPACE</t>
         </is>
       </c>
       <c r="C69" s="70" t="inlineStr">
         <is>
-          <t>\n</t>
+          <t>空格</t>
         </is>
       </c>
     </row>
@@ -1324,12 +1323,12 @@
       </c>
       <c r="B73" s="74" t="inlineStr">
         <is>
-          <t>WHITESPACE/SPACE</t>
+          <t>WORD/WRITE</t>
         </is>
       </c>
       <c r="C73" s="74" t="inlineStr">
         <is>
-          <t>空格</t>
+          <t>write</t>
         </is>
       </c>
     </row>
@@ -1339,12 +1338,12 @@
       </c>
       <c r="B74" s="75" t="inlineStr">
         <is>
-          <t>WORD/WRITE</t>
+          <t>PAIRDELIMITER/L_PARENTHESIS</t>
         </is>
       </c>
       <c r="C74" s="75" t="inlineStr">
         <is>
-          <t>write</t>
+          <t>(</t>
         </is>
       </c>
     </row>
@@ -1354,12 +1353,12 @@
       </c>
       <c r="B75" s="76" t="inlineStr">
         <is>
-          <t>PAIRDELIMITER/L_PARENTHESIS</t>
+          <t>IDENTIFIER</t>
         </is>
       </c>
       <c r="C75" s="76" t="inlineStr">
         <is>
-          <t>(</t>
+          <t>v1</t>
         </is>
       </c>
     </row>
@@ -1369,12 +1368,12 @@
       </c>
       <c r="B76" s="77" t="inlineStr">
         <is>
-          <t>IDENTIFIER</t>
+          <t>PAIRDELIMITER/R_PARENTHESIS</t>
         </is>
       </c>
       <c r="C76" s="77" t="inlineStr">
         <is>
-          <t>v1</t>
+          <t>)</t>
         </is>
       </c>
     </row>
@@ -1384,27 +1383,27 @@
       </c>
       <c r="B77" s="78" t="inlineStr">
         <is>
-          <t>PAIRDELIMITER/R_PARENTHESIS</t>
+          <t>ENDDELIMITER/SEMICOLON</t>
         </is>
       </c>
       <c r="C77" s="78" t="inlineStr">
         <is>
-          <t>)</t>
+          <t>;</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="79" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="B78" s="79" t="inlineStr">
         <is>
-          <t>ENDDELIMITER/SEMICOLON</t>
+          <t>WHITESPACE/NEW_LINE</t>
         </is>
       </c>
       <c r="C78" s="79" t="inlineStr">
         <is>
-          <t>;</t>
+          <t>\n</t>
         </is>
       </c>
     </row>
@@ -1414,12 +1413,12 @@
       </c>
       <c r="B79" s="80" t="inlineStr">
         <is>
-          <t>WHITESPACE/NEW_LINE</t>
+          <t>WORD/END</t>
         </is>
       </c>
       <c r="C79" s="80" t="inlineStr">
         <is>
-          <t>\n</t>
+          <t>end</t>
         </is>
       </c>
     </row>
@@ -1429,25 +1428,10 @@
       </c>
       <c r="B80" s="81" t="inlineStr">
         <is>
-          <t>WORD/END</t>
+          <t>PROGRAMEND</t>
         </is>
       </c>
       <c r="C80" s="81" t="inlineStr">
-        <is>
-          <t>end</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" s="82" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="B81" s="82" t="inlineStr">
-        <is>
-          <t>PROGRAMEND</t>
-        </is>
-      </c>
-      <c r="C81" s="82" t="inlineStr">
         <is>
           <t>.</t>
         </is>

</xml_diff>